<commit_message>
add bt report export
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -6,12 +6,13 @@
     <sheet name="应收账款-数量" sheetId="1" r:id="rId4"/>
     <sheet name="应收账款-收入" sheetId="2" r:id="rId5"/>
     <sheet name="Percent" sheetId="3" r:id="rId6"/>
+    <sheet name="ss" sheetId="4" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15" xml:space="preserve">
   <si>
     <t>Email</t>
   </si>
@@ -28,9 +29,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>实际或计划</t>
-  </si>
-  <si>
     <t>admin@ci.com</t>
   </si>
   <si>
@@ -40,6 +38,12 @@
     <t>应收账款-收入</t>
   </si>
   <si>
+    <t>deliveryNr</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
     <t>性别</t>
   </si>
   <si>
@@ -50,6 +54,9 @@
   </si>
   <si>
     <t>Percent</t>
+  </si>
+  <si>
+    <t>ss</t>
   </si>
 </sst>
 </file>
@@ -124,7 +131,6 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.589887640449438"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -143,19 +149,16 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
@@ -193,7 +196,6 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.589887640449438"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -212,19 +214,16 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
@@ -262,9 +261,11 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="5.289887640449439"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="5.289887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -284,24 +285,95 @@
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>39</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="true"/>
+  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
+  <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
+  <pageSetup/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
fix down kpi template ability
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -3,16 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="应收账款-数量" sheetId="1" r:id="rId4"/>
-    <sheet name="应收账款-收入" sheetId="2" r:id="rId5"/>
-    <sheet name="Percent" sheetId="3" r:id="rId6"/>
-    <sheet name="ss" sheetId="4" r:id="rId7"/>
+    <sheet name="总刀片寿命" sheetId="1" r:id="rId4"/>
+    <sheet name="换刀记录" sheetId="2" r:id="rId5"/>
+    <sheet name="总维修时间" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20" xml:space="preserve">
   <si>
     <t>Email</t>
   </si>
@@ -29,34 +28,49 @@
     <t>Value</t>
   </si>
   <si>
-    <t>admin@ci.com</t>
-  </si>
-  <si>
-    <t>应收账款-数量</t>
-  </si>
-  <si>
-    <t>应收账款-收入</t>
-  </si>
-  <si>
-    <t>deliveryNr</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>性别</t>
-  </si>
-  <si>
-    <t>国家</t>
-  </si>
-  <si>
-    <t>城市</t>
-  </si>
-  <si>
-    <t>Percent</t>
-  </si>
-  <si>
-    <t>ss</t>
+    <t>损坏状态</t>
+  </si>
+  <si>
+    <t>刀片分类</t>
+  </si>
+  <si>
+    <t>模具号</t>
+  </si>
+  <si>
+    <t>mj@leoni.com</t>
+  </si>
+  <si>
+    <t>总刀片寿命</t>
+  </si>
+  <si>
+    <t>损坏定义</t>
+  </si>
+  <si>
+    <t>项目</t>
+  </si>
+  <si>
+    <t>出库单号</t>
+  </si>
+  <si>
+    <t>换刀记录</t>
+  </si>
+  <si>
+    <t>设备编号</t>
+  </si>
+  <si>
+    <t>抢修人员</t>
+  </si>
+  <si>
+    <t>问题描述</t>
+  </si>
+  <si>
+    <t>送料方式</t>
+  </si>
+  <si>
+    <t>解决措施</t>
+  </si>
+  <si>
+    <t>总维修时间</t>
   </si>
 </sst>
 </file>
@@ -126,11 +140,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -149,16 +166,25 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
@@ -191,11 +217,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.489887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -214,16 +245,31 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
@@ -256,16 +302,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.289887640449439"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.289887640449439"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="7.489887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -285,95 +333,36 @@
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E2" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <sheetCalcPr fullCalcOnLoad="true"/>
-  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
-  <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
-  <pageSetup/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.289887640449439"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>

</xml_diff>